<commit_message>
Last modifications to User Stories and other documentation stuff
git-svn-id: https://euclid.esac.esa.int/svn/ESA/SOC/SOC-3-DEV/SOC-3-07-QLook/QPF/trunk@11926 463500fe-d6be-4184-9b20-47717e75ecac
</commit_message>
<xml_diff>
--- a/doc/QLA-QPF-UserStories-20150803.xlsx
+++ b/doc/QLA-QPF-UserStories-20150803.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="312">
   <si>
     <t>QLA Processing Framework User Stories</t>
   </si>
@@ -855,6 +855,108 @@
   </si>
   <si>
     <t>QLA-QPF-US-050.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-060.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-060.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-070.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-070.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-080.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-080.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-090.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-090.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-100.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-100.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-110.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-110.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-120.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-120.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-130.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-130.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-140.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-140.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-150.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-150.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-160.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-160.020</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-170.010</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-170.020</t>
+  </si>
+  <si>
+    <t>I can modify/adjust the configuration of the system for the next execution</t>
+  </si>
+  <si>
+    <t>have the configuration tool accessible from a Tools menu of the QPF HMI</t>
+  </si>
+  <si>
+    <t>I can easily access to it</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-070.030</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-070.040</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-070.050</t>
+  </si>
+  <si>
+    <t>These stories are the same as US-030.*.  Address any differences</t>
+  </si>
+  <si>
+    <t>have different channels where to get information about system actions</t>
+  </si>
+  <si>
+    <t>be able to tune the level of information I get from the system for every channel</t>
+  </si>
+  <si>
+    <t>I can adapt my needs</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1105,147 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1306,20 +1548,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1960,35 +2188,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:H38" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:H38" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A5:H38"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Scope" dataDxfId="49"/>
-    <tableColumn id="2" name="User Story ID" dataDxfId="48"/>
-    <tableColumn id="3" name="Contact" dataDxfId="47"/>
-    <tableColumn id="4" name="What" dataDxfId="46"/>
-    <tableColumn id="5" name="Why" dataDxfId="45"/>
-    <tableColumn id="6" name="Input" dataDxfId="44"/>
-    <tableColumn id="7" name="Output" dataDxfId="43"/>
-    <tableColumn id="8" name="Notes" dataDxfId="42"/>
+    <tableColumn id="1" name="Scope" dataDxfId="67"/>
+    <tableColumn id="2" name="User Story ID" dataDxfId="66"/>
+    <tableColumn id="3" name="Contact" dataDxfId="65"/>
+    <tableColumn id="4" name="What" dataDxfId="64"/>
+    <tableColumn id="5" name="Why" dataDxfId="63"/>
+    <tableColumn id="6" name="Input" dataDxfId="62"/>
+    <tableColumn id="7" name="Output" dataDxfId="61"/>
+    <tableColumn id="8" name="Notes" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="QPFUserStories" displayName="QPFUserStories" ref="A5:I37" headerRowDxfId="41" dataDxfId="19" totalsRowDxfId="40">
-  <autoFilter ref="A5:I37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="QPFUserStories" displayName="QPFUserStories" ref="A5:I64" headerRowDxfId="59" dataDxfId="39" totalsRowDxfId="58">
+  <autoFilter ref="A5:I64"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Id" totalsRowLabel="Total" dataDxfId="28" totalsRowDxfId="39"/>
-    <tableColumn id="9" name="Class" dataDxfId="27" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Theme" dataDxfId="26" totalsRowDxfId="37"/>
-    <tableColumn id="3" name="As a/an" dataDxfId="25" totalsRowDxfId="36"/>
-    <tableColumn id="4" name="I want to" dataDxfId="24" totalsRowDxfId="35"/>
-    <tableColumn id="5" name="so that" dataDxfId="23" totalsRowDxfId="34"/>
-    <tableColumn id="6" name="Notes" dataDxfId="22" totalsRowDxfId="33"/>
-    <tableColumn id="7" name="Priority" dataDxfId="21" totalsRowDxfId="32"/>
-    <tableColumn id="8" name="Status" totalsRowFunction="count" dataDxfId="20" totalsRowDxfId="31"/>
+    <tableColumn id="1" name="Id" totalsRowLabel="Total" dataDxfId="48" totalsRowDxfId="57"/>
+    <tableColumn id="9" name="Class" dataDxfId="47" totalsRowDxfId="56"/>
+    <tableColumn id="2" name="Theme" dataDxfId="46" totalsRowDxfId="55"/>
+    <tableColumn id="3" name="As a/an" dataDxfId="45" totalsRowDxfId="54"/>
+    <tableColumn id="4" name="I want to" dataDxfId="44" totalsRowDxfId="53"/>
+    <tableColumn id="5" name="so that" dataDxfId="43" totalsRowDxfId="52"/>
+    <tableColumn id="6" name="Notes" dataDxfId="42" totalsRowDxfId="51"/>
+    <tableColumn id="7" name="Priority" dataDxfId="41" totalsRowDxfId="50"/>
+    <tableColumn id="8" name="Status" totalsRowFunction="count" dataDxfId="40" totalsRowDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3181,10 +3409,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,10 +3420,10 @@
     <col min="1" max="1" width="20.5703125" style="7" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="60.7109375" style="7" customWidth="1"/>
     <col min="8" max="9" width="11.7109375" style="7" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="7"/>
   </cols>
@@ -3656,49 +3884,53 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>49</v>
+      <c r="E24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>302</v>
       </c>
       <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>225</v>
+        <v>279</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C25" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>51</v>
+      <c r="E25" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>304</v>
       </c>
       <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>217</v>
@@ -3710,127 +3942,141 @@
         <v>24</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>199</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C27" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>55</v>
+      <c r="E27" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>200</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C28" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C29" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>204</v>
+      <c r="E29" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>212</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C30" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="G30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C31" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="G31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>217</v>
@@ -3842,58 +4088,62 @@
         <v>24</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>209</v>
+        <v>50</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>233</v>
+        <v>282</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>211</v>
+      <c r="E33" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>234</v>
+        <v>283</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C34" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>214</v>
+      <c r="E34" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>217</v>
@@ -3904,41 +4154,578 @@
       <c r="D35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C37" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A6:I37">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A6:I64">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$B6="Epic"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New user stories (new revision)
git-svn-id: https://euclid.esac.esa.int/svn/ESA/SOC/SOC-3-DEV/SOC-3-07-QLook/QPF/trunk@11946 463500fe-d6be-4184-9b20-47717e75ecac
</commit_message>
<xml_diff>
--- a/doc/QLA-QPF-UserStories-20150803.xlsx
+++ b/doc/QLA-QPF-UserStories-20150803.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11340" windowHeight="5265" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11340" windowHeight="5265"/>
   </bookViews>
   <sheets>
     <sheet name="QLA User Stories" sheetId="3" r:id="rId1"/>
     <sheet name="QPF US" sheetId="1" r:id="rId2"/>
     <sheet name="QPF Components Internal IF" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="priorities">'QPF US'!$M$2:$M$4</definedName>
+    <definedName name="statuses">'QPF US'!$O$2:$O$4</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="351">
   <si>
     <t>QLA Processing Framework User Stories</t>
   </si>
@@ -728,15 +732,6 @@
     <t>QLA-QPF-US-170</t>
   </si>
   <si>
-    <t>QLA-QPF-US-180</t>
-  </si>
-  <si>
-    <t>QLA-QPF-US-190</t>
-  </si>
-  <si>
-    <t>QLA-QPF-US-200</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
@@ -809,9 +804,6 @@
     <t>I can select one of them to be executed interactively on a set of data</t>
   </si>
   <si>
-    <t>Last Update 20150806</t>
-  </si>
-  <si>
     <t>QLA-QPF-US-040.010</t>
   </si>
   <si>
@@ -908,15 +900,9 @@
     <t>QLA-QPF-US-140.010</t>
   </si>
   <si>
-    <t>QLA-QPF-US-140.020</t>
-  </si>
-  <si>
     <t>QLA-QPF-US-150.010</t>
   </si>
   <si>
-    <t>QLA-QPF-US-150.020</t>
-  </si>
-  <si>
     <t>QLA-QPF-US-160.010</t>
   </si>
   <si>
@@ -957,13 +943,148 @@
   </si>
   <si>
     <t>I can adapt my needs</t>
+  </si>
+  <si>
+    <t>see a panel with all alerts that the system detects</t>
+  </si>
+  <si>
+    <t>I can choose any of them and check its information</t>
+  </si>
+  <si>
+    <t>get a menu of actions on a selected alert</t>
+  </si>
+  <si>
+    <t>I can get several information aspects and perform actions accordingly</t>
+  </si>
+  <si>
+    <t>Same as QLA-QPF-US-090.010</t>
+  </si>
+  <si>
+    <t>be able to select one of these alerts</t>
+  </si>
+  <si>
+    <t>I can check the data that was the source of the alert</t>
+  </si>
+  <si>
+    <t>have available a panel with status information on the different tasks</t>
+  </si>
+  <si>
+    <t>I can see at any time the processing status of the system</t>
+  </si>
+  <si>
+    <t>have a place where the system stores the processing status of the different tasks</t>
+  </si>
+  <si>
+    <t>in case of system failure, I can see what tasks were not executed</t>
+  </si>
+  <si>
+    <t>be able to stop the system and re-start it at any time</t>
+  </si>
+  <si>
+    <t>I can perform any system maintenance activities</t>
+  </si>
+  <si>
+    <t>be able to restart the system at the state that it was before stopping it</t>
+  </si>
+  <si>
+    <t>the system executes any task that was scheduled but not executed</t>
+  </si>
+  <si>
+    <t>have a list of the different processing tasks executed, in execution or scheduled</t>
+  </si>
+  <si>
+    <t>I can pause a running task</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-130.030</t>
+  </si>
+  <si>
+    <t>QLA-QPF-US-130.040</t>
+  </si>
+  <si>
+    <t>I can resume a paused task</t>
+  </si>
+  <si>
+    <t>I can completelt stop a running task</t>
+  </si>
+  <si>
+    <t>I can remove a task (that was running, paused, waiting or stopped)</t>
+  </si>
+  <si>
+    <t>have a user-defined repository (directory) selector</t>
+  </si>
+  <si>
+    <t>the system takes the data from that directory and injects it into the system</t>
+  </si>
+  <si>
+    <t>have a browser for the data stored in the local (temporary) archive</t>
+  </si>
+  <si>
+    <t>I can select a data set and open it with an external tool</t>
+  </si>
+  <si>
+    <t>have a list of algorithms/procedures that are executed on input data files</t>
+  </si>
+  <si>
+    <t>I can select one of them to be run on th selected dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can select a dataset for reprocessing </t>
+  </si>
+  <si>
+    <t>have all the system information stored in a DB, to be permanently up-to-date</t>
+  </si>
+  <si>
+    <t>have a DB browser</t>
+  </si>
+  <si>
+    <t>I can browse all the DB tables stored by the system</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Status are:</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Withdrawn</t>
+  </si>
+  <si>
+    <t>Last Update 20150812</t>
+  </si>
+  <si>
+    <t>To be implemented</t>
+  </si>
+  <si>
+    <t>Removed from the list</t>
+  </si>
+  <si>
+    <t>All dependant tasks are implemented and tested</t>
+  </si>
+  <si>
+    <t>Priorities:</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,6 +1109,20 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1061,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1100,16 +1235,119 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1123,7 +1361,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1135,11 +1387,22 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1149,214 +1412,21 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Corbel"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1392,8 +1462,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Corbel"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -1409,127 +1479,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <name val="Corbel"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -1579,8 +1530,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Corbel"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -1613,8 +1564,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Corbel"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -1647,8 +1598,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Corbel"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -1681,8 +1632,8 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Corbel"/>
-        <scheme val="none"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -1704,12 +1655,114 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Corbel"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Corbel"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -1903,6 +1956,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2188,35 +2246,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:H38" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:H38" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A5:H38"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Scope" dataDxfId="67"/>
-    <tableColumn id="2" name="User Story ID" dataDxfId="66"/>
-    <tableColumn id="3" name="Contact" dataDxfId="65"/>
-    <tableColumn id="4" name="What" dataDxfId="64"/>
-    <tableColumn id="5" name="Why" dataDxfId="63"/>
-    <tableColumn id="6" name="Input" dataDxfId="62"/>
-    <tableColumn id="7" name="Output" dataDxfId="61"/>
-    <tableColumn id="8" name="Notes" dataDxfId="60"/>
+    <tableColumn id="1" name="Scope" dataDxfId="52"/>
+    <tableColumn id="2" name="User Story ID" dataDxfId="51"/>
+    <tableColumn id="3" name="Contact" dataDxfId="50"/>
+    <tableColumn id="4" name="What" dataDxfId="49"/>
+    <tableColumn id="5" name="Why" dataDxfId="48"/>
+    <tableColumn id="6" name="Input" dataDxfId="47"/>
+    <tableColumn id="7" name="Output" dataDxfId="46"/>
+    <tableColumn id="8" name="Notes" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="QPFUserStories" displayName="QPFUserStories" ref="A5:I64" headerRowDxfId="59" dataDxfId="39" totalsRowDxfId="58">
-  <autoFilter ref="A5:I64"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Id" totalsRowLabel="Total" dataDxfId="48" totalsRowDxfId="57"/>
-    <tableColumn id="9" name="Class" dataDxfId="47" totalsRowDxfId="56"/>
-    <tableColumn id="2" name="Theme" dataDxfId="46" totalsRowDxfId="55"/>
-    <tableColumn id="3" name="As a/an" dataDxfId="45" totalsRowDxfId="54"/>
-    <tableColumn id="4" name="I want to" dataDxfId="44" totalsRowDxfId="53"/>
-    <tableColumn id="5" name="so that" dataDxfId="43" totalsRowDxfId="52"/>
-    <tableColumn id="6" name="Notes" dataDxfId="42" totalsRowDxfId="51"/>
-    <tableColumn id="7" name="Priority" dataDxfId="41" totalsRowDxfId="50"/>
-    <tableColumn id="8" name="Status" totalsRowFunction="count" dataDxfId="40" totalsRowDxfId="49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="QPFUserStories" displayName="QPFUserStories" ref="A6:J62" headerRowDxfId="44" dataDxfId="43" totalsRowDxfId="42">
+  <autoFilter ref="A6:J62"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Id" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="9" name="Class" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Theme" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="As a/an" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="I want to" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="so that" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Notes" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="10" name="P" dataDxfId="19" totalsRowDxfId="21">
+      <calculatedColumnFormula>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Priority" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="8" name="Status" totalsRowFunction="count" dataDxfId="4" totalsRowDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2525,7 +2586,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -3409,10 +3470,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3424,81 +3488,106 @@
     <col min="5" max="5" width="72.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.85546875" style="7" customWidth="1"/>
     <col min="7" max="7" width="60.7109375" style="7" customWidth="1"/>
-    <col min="8" max="9" width="11.7109375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="7"/>
+    <col min="8" max="8" width="2.7109375" style="7" customWidth="1"/>
+    <col min="9" max="10" width="11.7109375" style="7" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" style="7"/>
+    <col min="15" max="15" width="12.42578125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" style="7" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H6" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>11</v>
@@ -3507,44 +3596,64 @@
         <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>242</v>
+        <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="H7" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>20</v>
+        <v>239</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>21</v>
+        <v>237</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="H8" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>11</v>
@@ -3553,42 +3662,64 @@
         <v>17</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>244</v>
+        <v>20</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>245</v>
+        <v>21</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H9" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="F10" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H10" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>12</v>
@@ -3596,22 +3727,30 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>248</v>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>12</v>
@@ -3620,21 +3759,29 @@
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>12</v>
@@ -3643,21 +3790,29 @@
         <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>12</v>
@@ -3666,23 +3821,29 @@
         <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>12</v>
@@ -3691,21 +3852,31 @@
         <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H15" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>12</v>
@@ -3713,20 +3884,30 @@
       <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>16</v>
+      <c r="E16" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>12</v>
@@ -3734,22 +3915,30 @@
       <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>265</v>
+      <c r="E17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>12</v>
@@ -3758,21 +3947,29 @@
         <v>13</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>12</v>
@@ -3781,42 +3978,60 @@
         <v>13</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>222</v>
+        <v>263</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>265</v>
       </c>
       <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>276</v>
+        <v>222</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>12</v>
@@ -3824,24 +4039,30 @@
       <c r="D21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="B22" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>12</v>
@@ -3850,67 +4071,95 @@
         <v>17</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="H22" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H23" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>302</v>
+      <c r="F24" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>23</v>
@@ -3919,67 +4168,91 @@
         <v>24</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>303</v>
+        <v>25</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C26" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>49</v>
+      <c r="E26" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>298</v>
       </c>
       <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C27" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>23</v>
@@ -3988,23 +4261,31 @@
         <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="H28" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>23</v>
@@ -4013,23 +4294,31 @@
         <v>24</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="H29" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>23</v>
@@ -4038,23 +4327,31 @@
         <v>24</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="H30" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>23</v>
@@ -4063,67 +4360,95 @@
         <v>24</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="H31" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>225</v>
+        <v>301</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H32" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C33" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>23</v>
@@ -4132,63 +4457,93 @@
         <v>24</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>311</v>
+        <v>51</v>
       </c>
       <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>226</v>
+        <v>279</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C35" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>284</v>
+        <v>226</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H36" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>23</v>
@@ -4196,60 +4551,94 @@
       <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C38" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>286</v>
+        <v>227</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C39" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H39" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>23</v>
@@ -4257,58 +4646,94 @@
       <c r="D40" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="H40" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>228</v>
+        <v>283</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>202</v>
+      <c r="E41" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>312</v>
       </c>
       <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>288</v>
+        <v>228</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C42" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="E42" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>202</v>
+      </c>
       <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>23</v>
@@ -4316,60 +4741,94 @@
       <c r="D43" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>314</v>
+      </c>
       <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C44" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E44" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>290</v>
+        <v>229</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C45" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E45" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H45" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>23</v>
@@ -4377,58 +4836,92 @@
       <c r="D46" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>318</v>
+      </c>
       <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>230</v>
+        <v>287</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C47" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>206</v>
+      <c r="E47" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H47" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>292</v>
+        <v>230</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C48" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="E48" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>206</v>
+      </c>
       <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>23</v>
@@ -4436,39 +4929,61 @@
       <c r="D49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>322</v>
+      </c>
       <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>231</v>
+        <v>289</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C50" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>208</v>
+      <c r="E50" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="G50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H50" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>23</v>
@@ -4476,18 +4991,30 @@
       <c r="D51" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="G51" s="20"/>
+      <c r="H51" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>23</v>
@@ -4495,15 +5022,27 @@
       <c r="D52" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E52" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="G52" s="20"/>
+      <c r="H52" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>217</v>
@@ -4515,19 +5054,29 @@
         <v>24</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H53" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>23</v>
@@ -4535,77 +5084,123 @@
       <c r="D54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>329</v>
+      </c>
       <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>297</v>
+        <v>232</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C55" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="E55" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>210</v>
+      </c>
       <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H55" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>233</v>
+        <v>291</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C56" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>211</v>
+      <c r="E56" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>2</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>298</v>
+        <v>233</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C57" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="E57" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>211</v>
+      </c>
       <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H57" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>23</v>
@@ -4613,58 +5208,92 @@
       <c r="D58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>334</v>
+      </c>
       <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>234</v>
+        <v>293</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C59" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>214</v>
+      <c r="E59" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>333</v>
       </c>
       <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C60" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="E60" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>214</v>
+      </c>
       <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="7">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>23</v>
@@ -4672,63 +5301,107 @@
       <c r="D61" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="E62" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>337</v>
+      </c>
       <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H62" s="5">
+        <f>MATCH(QPFUserStories[[#This Row],[Priority]],{"High";"Medium";"Low"},0)</f>
+        <v>3</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="D63" s="5"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>24</v>
-      </c>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="D64" s="5"/>
       <c r="G64" s="5"/>
     </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A6:I64">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$B6="Epic"</formula>
+  <conditionalFormatting sqref="A7:G62">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>$B7="Epic"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J62">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>J7="Withdrawn"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>J7="Open"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>J7="Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H62">
+    <cfRule type="iconSet" priority="8">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I62">
+      <formula1>priorities</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J62">
+      <formula1>statuses</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>